<commit_message>
add change point, climatological period cal
</commit_message>
<xml_diff>
--- a/results/stations/Nguru/Nguru.xlsx
+++ b/results/stations/Nguru/Nguru.xlsx
@@ -16,12 +16,17 @@
     <sheet name="Chara_spei12" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Trends" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Drought_Total_Count" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Homogeneity Test" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Change Points Prec" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Change Points Tmin" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Change Points Tmax" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Climatological Analysis" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -240,6 +245,84 @@
   </si>
   <si>
     <t xml:space="preserve">spei12_extreme_total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_Statistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternative_Hypothesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical_Values_1pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical_Values_5pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Critical_Values_10pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Augmented Dickey-Fuller Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stationary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changepoint_Locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter_Estimates1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter_Estimates2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penalty_Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PELT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tmin_Trend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tmax_Trend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre_Trend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tmin_Sen_Slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tmax_Sen_Slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre_Sen_Slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accelerated Climate Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Climate Change Onset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
   </si>
 </sst>
 </file>
@@ -50072,6 +50155,3379 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-23.1618562856287</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>77.1857142857143</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>125.266666666667</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>82.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>22</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>83.6857142857143</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>124.1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>34</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>99.3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>39</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>81.0857142857143</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>46</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>74.9428571428571</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>52</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>58</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>70.1857142857143</v>
+      </c>
+      <c r="D11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>65</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>76.1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>70</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>82.75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>75</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>51.3428571428571</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>82</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>41.1166666666667</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>87</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>84.6285714285714</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>94</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>82.4285714285714</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>99</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>71.3166666666667</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>105</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>77.9333333333333</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>111</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>69.6428571428571</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>118</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>124</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>87.2333333333333</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>130</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>74.8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>135</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>68.3285714285714</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>141</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>75.58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>147</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>36.8714285714286</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>154</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>84.66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>160</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>72.85</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>166</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>52.06</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>171</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>82.4428571428571</v>
+      </c>
+      <c r="D30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>178</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>55.9857142857143</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>183</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>190</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>72.3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>196</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>64.6857142857143</v>
+      </c>
+      <c r="D34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>202</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>208</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>99.4714285714286</v>
+      </c>
+      <c r="D36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>214</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>65</v>
+      </c>
+      <c r="D37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>219</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>75.7833333333333</v>
+      </c>
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>226</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>68.3857142857143</v>
+      </c>
+      <c r="D39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>232</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>74.3428571428571</v>
+      </c>
+      <c r="D40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>238</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>83.3285714285714</v>
+      </c>
+      <c r="D41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>244</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>65.1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>250</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>84.5285714285714</v>
+      </c>
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>255</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>61.4285714285714</v>
+      </c>
+      <c r="D44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>261</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>99.6571428571429</v>
+      </c>
+      <c r="D45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>267</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>63.1285714285714</v>
+      </c>
+      <c r="D46" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>274</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>92.8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>280</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>72.7571428571429</v>
+      </c>
+      <c r="D48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>285</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>77.0571428571429</v>
+      </c>
+      <c r="D49" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>291</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>75.3142857142857</v>
+      </c>
+      <c r="D50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>298</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>66.0428571428571</v>
+      </c>
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E51" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>304</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" t="n">
+        <v>93.1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>309</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>75.8714285714286</v>
+      </c>
+      <c r="D53" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>316</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>109.428571428571</v>
+      </c>
+      <c r="D54" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>322</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>78.9285714285714</v>
+      </c>
+      <c r="D55" t="s">
+        <v>86</v>
+      </c>
+      <c r="E55" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F55" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>328</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>70.3142857142857</v>
+      </c>
+      <c r="D56" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F56" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>333</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>63.8428571428571</v>
+      </c>
+      <c r="D57" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>339</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>82.4142857142857</v>
+      </c>
+      <c r="D58" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>346</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>87.4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>351</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>99.8285714285714</v>
+      </c>
+      <c r="D60" t="s">
+        <v>86</v>
+      </c>
+      <c r="E60" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F60" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>358</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>84.5714285714286</v>
+      </c>
+      <c r="D61" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>364</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>86</v>
+      </c>
+      <c r="E62" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>369</v>
+      </c>
+      <c r="B63" t="n">
+        <v>5702.41551020408</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
+        <v>86</v>
+      </c>
+      <c r="E63" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F63" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>375</v>
+      </c>
+      <c r="B64" t="n">
+        <v>17855.8988888889</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" t="s">
+        <v>86</v>
+      </c>
+      <c r="E64" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F64" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>382</v>
+      </c>
+      <c r="B65" t="n">
+        <v>6593.67142857143</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F65" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>387</v>
+      </c>
+      <c r="B66" t="n">
+        <v>4305.61836734694</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>86</v>
+      </c>
+      <c r="E66" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>394</v>
+      </c>
+      <c r="B67" t="n">
+        <v>15951.5633333333</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>86</v>
+      </c>
+      <c r="E67" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>400</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3031.644</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>86</v>
+      </c>
+      <c r="E68" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F68" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>406</v>
+      </c>
+      <c r="B69" t="n">
+        <v>2846.3812244898</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="s">
+        <v>86</v>
+      </c>
+      <c r="E69" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F69" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>411</v>
+      </c>
+      <c r="B70" t="n">
+        <v>6348.37102040816</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
+        <v>86</v>
+      </c>
+      <c r="E70" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>418</v>
+      </c>
+      <c r="B71" t="n">
+        <v>2178.81</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>86</v>
+      </c>
+      <c r="E71" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>423</v>
+      </c>
+      <c r="B72" t="n">
+        <v>3330.39265306122</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E72" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>430</v>
+      </c>
+      <c r="B73" t="n">
+        <v>5404.92</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>86</v>
+      </c>
+      <c r="E73" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F73" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>436</v>
+      </c>
+      <c r="B74" t="n">
+        <v>4744.35583333333</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
+        <v>86</v>
+      </c>
+      <c r="E74" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>442</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1486.47673469388</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>86</v>
+      </c>
+      <c r="E75" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>447</v>
+      </c>
+      <c r="B76" t="n">
+        <v>1563.81472222222</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
+        <v>86</v>
+      </c>
+      <c r="E76" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F76" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>454</v>
+      </c>
+      <c r="B77" t="n">
+        <v>7893.90775510204</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="s">
+        <v>86</v>
+      </c>
+      <c r="E77" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>459</v>
+      </c>
+      <c r="B78" t="n">
+        <v>4985.7506122449</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>86</v>
+      </c>
+      <c r="E78" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F78" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>466</v>
+      </c>
+      <c r="B79" t="n">
+        <v>2415.72805555556</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" t="s">
+        <v>86</v>
+      </c>
+      <c r="E79" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>471</v>
+      </c>
+      <c r="B80" t="n">
+        <v>6258.87888888889</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0</v>
+      </c>
+      <c r="D80" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>478</v>
+      </c>
+      <c r="B81" t="n">
+        <v>4608.83959183673</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
+      <c r="D81" t="s">
+        <v>86</v>
+      </c>
+      <c r="E81" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>483</v>
+      </c>
+      <c r="B82" t="n">
+        <v>4611.52666666667</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F82" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>490</v>
+      </c>
+      <c r="B83" t="n">
+        <v>5214.83222222222</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" t="s">
+        <v>86</v>
+      </c>
+      <c r="E83" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F83" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>495</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2864.00666666667</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="s">
+        <v>86</v>
+      </c>
+      <c r="E84" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>502</v>
+      </c>
+      <c r="B85" t="n">
+        <v>5176.66204081633</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
+        <v>86</v>
+      </c>
+      <c r="E85" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>507</v>
+      </c>
+      <c r="B86" t="n">
+        <v>1842.3296</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F86" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>514</v>
+      </c>
+      <c r="B87" t="n">
+        <v>955.413469387755</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="s">
+        <v>86</v>
+      </c>
+      <c r="E87" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F87" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>519</v>
+      </c>
+      <c r="B88" t="n">
+        <v>3172.1544</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="s">
+        <v>86</v>
+      </c>
+      <c r="E88" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>526</v>
+      </c>
+      <c r="B89" t="n">
+        <v>3847.10916666667</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0</v>
+      </c>
+      <c r="D89" t="s">
+        <v>86</v>
+      </c>
+      <c r="E89" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F89" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>531</v>
+      </c>
+      <c r="B90" t="n">
+        <v>666.3064</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+      <c r="D90" t="s">
+        <v>86</v>
+      </c>
+      <c r="E90" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F90" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>538</v>
+      </c>
+      <c r="B91" t="n">
+        <v>7367.15387755102</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" t="s">
+        <v>86</v>
+      </c>
+      <c r="E91" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F91" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>543</v>
+      </c>
+      <c r="B92" t="n">
+        <v>5448.27551020408</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="s">
+        <v>86</v>
+      </c>
+      <c r="E92" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F92" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>550</v>
+      </c>
+      <c r="B93" t="n">
+        <v>3194.46</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0</v>
+      </c>
+      <c r="D93" t="s">
+        <v>86</v>
+      </c>
+      <c r="E93" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F93" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>555</v>
+      </c>
+      <c r="B94" t="n">
+        <v>5563.14857142857</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" t="s">
+        <v>86</v>
+      </c>
+      <c r="E94" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F94" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>562</v>
+      </c>
+      <c r="B95" t="n">
+        <v>2751.04693877551</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" t="s">
+        <v>86</v>
+      </c>
+      <c r="E95" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F95" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>567</v>
+      </c>
+      <c r="B96" t="n">
+        <v>4359.31666666667</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" t="s">
+        <v>86</v>
+      </c>
+      <c r="E96" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F96" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>574</v>
+      </c>
+      <c r="B97" t="n">
+        <v>9330.92204081633</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0</v>
+      </c>
+      <c r="D97" t="s">
+        <v>86</v>
+      </c>
+      <c r="E97" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F97" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>579</v>
+      </c>
+      <c r="B98" t="n">
+        <v>3922.6</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0</v>
+      </c>
+      <c r="D98" t="s">
+        <v>86</v>
+      </c>
+      <c r="E98" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F98" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>586</v>
+      </c>
+      <c r="B99" t="n">
+        <v>3292.52805555556</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" t="s">
+        <v>86</v>
+      </c>
+      <c r="E99" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F99" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>591</v>
+      </c>
+      <c r="B100" t="n">
+        <v>3203.21551020408</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" t="s">
+        <v>86</v>
+      </c>
+      <c r="E100" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F100" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>598</v>
+      </c>
+      <c r="B101" t="n">
+        <v>4847.08816326531</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D101" t="s">
+        <v>86</v>
+      </c>
+      <c r="E101" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F101" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>603</v>
+      </c>
+      <c r="B102" t="n">
+        <v>7039.63918367347</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0</v>
+      </c>
+      <c r="D102" t="s">
+        <v>86</v>
+      </c>
+      <c r="E102" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F102" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>610</v>
+      </c>
+      <c r="B103" t="n">
+        <v>3782.77714285714</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0</v>
+      </c>
+      <c r="D103" t="s">
+        <v>86</v>
+      </c>
+      <c r="E103" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F103" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>615</v>
+      </c>
+      <c r="B104" t="n">
+        <v>5773.1306122449</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0</v>
+      </c>
+      <c r="D104" t="s">
+        <v>86</v>
+      </c>
+      <c r="E104" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F104" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>622</v>
+      </c>
+      <c r="B105" t="n">
+        <v>3179.19632653061</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0</v>
+      </c>
+      <c r="D105" t="s">
+        <v>86</v>
+      </c>
+      <c r="E105" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F105" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>627</v>
+      </c>
+      <c r="B106" t="n">
+        <v>6704.96816326531</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0</v>
+      </c>
+      <c r="D106" t="s">
+        <v>86</v>
+      </c>
+      <c r="E106" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F106" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>634</v>
+      </c>
+      <c r="B107" t="n">
+        <v>3690.47918367347</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0</v>
+      </c>
+      <c r="D107" t="s">
+        <v>86</v>
+      </c>
+      <c r="E107" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F107" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>639</v>
+      </c>
+      <c r="B108" t="n">
+        <v>5944.56571428571</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0</v>
+      </c>
+      <c r="D108" t="s">
+        <v>86</v>
+      </c>
+      <c r="E108" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F108" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>646</v>
+      </c>
+      <c r="B109" t="n">
+        <v>6253.99673469388</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" t="s">
+        <v>86</v>
+      </c>
+      <c r="E109" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F109" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>651</v>
+      </c>
+      <c r="B110" t="n">
+        <v>5800.10530612245</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0</v>
+      </c>
+      <c r="D110" t="s">
+        <v>86</v>
+      </c>
+      <c r="E110" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F110" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>658</v>
+      </c>
+      <c r="B111" t="n">
+        <v>6123.83551020408</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" t="s">
+        <v>86</v>
+      </c>
+      <c r="E111" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F111" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>663</v>
+      </c>
+      <c r="B112" t="n">
+        <v>3130.79387755102</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0</v>
+      </c>
+      <c r="D112" t="s">
+        <v>86</v>
+      </c>
+      <c r="E112" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F112" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>670</v>
+      </c>
+      <c r="B113" t="n">
+        <v>5832.58571428571</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0</v>
+      </c>
+      <c r="D113" t="s">
+        <v>86</v>
+      </c>
+      <c r="E113" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F113" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>675</v>
+      </c>
+      <c r="B114" t="n">
+        <v>4009.02775510204</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0</v>
+      </c>
+      <c r="D114" t="s">
+        <v>86</v>
+      </c>
+      <c r="E114" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F114" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>682</v>
+      </c>
+      <c r="B115" t="n">
+        <v>8729.97346938776</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0</v>
+      </c>
+      <c r="D115" t="s">
+        <v>86</v>
+      </c>
+      <c r="E115" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F115" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>687</v>
+      </c>
+      <c r="B116" t="n">
+        <v>6043.82775510204</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0</v>
+      </c>
+      <c r="D116" t="s">
+        <v>86</v>
+      </c>
+      <c r="E116" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F116" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>694</v>
+      </c>
+      <c r="B117" t="n">
+        <v>4292.62979591837</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0</v>
+      </c>
+      <c r="D117" t="s">
+        <v>86</v>
+      </c>
+      <c r="E117" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F117" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>699</v>
+      </c>
+      <c r="B118" t="n">
+        <v>4729.14244897959</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0</v>
+      </c>
+      <c r="D118" t="s">
+        <v>86</v>
+      </c>
+      <c r="E118" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F118" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>706</v>
+      </c>
+      <c r="B119" t="n">
+        <v>5896.85836734694</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" t="s">
+        <v>86</v>
+      </c>
+      <c r="E119" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F119" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>711</v>
+      </c>
+      <c r="B120" t="n">
+        <v>6133.43714285714</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0</v>
+      </c>
+      <c r="D120" t="s">
+        <v>86</v>
+      </c>
+      <c r="E120" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F120" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>718</v>
+      </c>
+      <c r="B121" t="n">
+        <v>4534.62204081633</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" t="s">
+        <v>86</v>
+      </c>
+      <c r="E121" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F121" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>720</v>
+      </c>
+      <c r="B122" t="n">
+        <v>6702.52204081633</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0</v>
+      </c>
+      <c r="D122" t="s">
+        <v>86</v>
+      </c>
+      <c r="E122" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F122" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="n">
+        <v>18</v>
+      </c>
+      <c r="C2" t="n">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>19.18</v>
+      </c>
+      <c r="C3" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>16</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20.0230769230769</v>
+      </c>
+      <c r="C4" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20.1496815286624</v>
+      </c>
+      <c r="C5" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>44</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20.5633333333333</v>
+      </c>
+      <c r="C6" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>46</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20.5885714285714</v>
+      </c>
+      <c r="C7" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>203</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20.6524390243902</v>
+      </c>
+      <c r="C8" t="n">
+        <v>21.9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>205</v>
+      </c>
+      <c r="B9" t="n">
+        <v>19.91</v>
+      </c>
+      <c r="C9" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>235</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20.7483870967742</v>
+      </c>
+      <c r="C10" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>237</v>
+      </c>
+      <c r="B11" t="n">
+        <v>21.8</v>
+      </c>
+      <c r="C11" t="n">
+        <v>22.6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>307</v>
+      </c>
+      <c r="B12" t="n">
+        <v>17.75</v>
+      </c>
+      <c r="C12" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>309</v>
+      </c>
+      <c r="B13" t="n">
+        <v>21.3725806451613</v>
+      </c>
+      <c r="C13" t="n">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>391</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20.7666666666667</v>
+      </c>
+      <c r="C14" t="n">
+        <v>16.765</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>393</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>10.4196</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>403</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>16.2463905325444</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>405</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15.3898884336079</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>591</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>14.6436555555556</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>593</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>18.645012244898</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>619</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>17.4734696609161</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>621</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>22.1769</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>627</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>16.3212070759625</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>629</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>14.7753846153846</v>
+      </c>
+      <c r="D23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>691</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>10.9791666666667</v>
+      </c>
+      <c r="D24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>693</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>15.3161836628512</v>
+      </c>
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>720</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>15.3851851851852</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" t="n">
+        <v>35.23</v>
+      </c>
+      <c r="C2" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B3" t="n">
+        <v>34.5378048780488</v>
+      </c>
+      <c r="C3" t="n">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>94</v>
+      </c>
+      <c r="B4" t="n">
+        <v>34.8688102893891</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30.3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>96</v>
+      </c>
+      <c r="B5" t="n">
+        <v>35.4670103092784</v>
+      </c>
+      <c r="C5" t="n">
+        <v>41.4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>407</v>
+      </c>
+      <c r="B6" t="n">
+        <v>35.4069565217391</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8.2801</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>409</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8.51259518143961</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>603</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10.5336574270324</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>605</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>10.2008704431927</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>720</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10.2778646502836</v>
+      </c>
+      <c r="D10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" t="n">
+        <v>26.3170048480404</v>
+      </c>
+      <c r="F10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0146323125809431</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-0.0487363673746586</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0300434119999409</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.00104166666666668</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.00444444444444451</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.0502351820468903</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0132130477577448</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.0257108453661203</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.00231481481481481</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.00056022848534305</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-0.00249394541606307</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0379691310226917</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0400443635880947</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.00348837209302326</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>

</xml_diff>